<commit_message>
feat: update template capacidad term pos
</commit_message>
<xml_diff>
--- a/boot/src/main/resources/xlsx/mantenimientosgenerales/capacidadTerminalPOS.xlsx
+++ b/boot/src/main/resources/xlsx/mantenimientosgenerales/capacidadTerminalPOS.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E34725A2-CCF0-4B7D-9FF0-7E894F51DE25}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="14865" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="14865" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -71,7 +69,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,7 +375,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -469,23 +467,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -521,23 +502,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -713,7 +677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
@@ -723,7 +687,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="60" customWidth="1"/>
+    <col min="5" max="5" width="72.5703125" customWidth="1"/>
     <col min="6" max="6" width="36.5703125" customWidth="1"/>
     <col min="7" max="7" width="67.140625" customWidth="1"/>
     <col min="8" max="8" width="62.42578125" customWidth="1"/>

</xml_diff>